<commit_message>
OPTIONAL SORTING AND FREE_SHIPMENT
</commit_message>
<xml_diff>
--- a/keywords.xlsx
+++ b/keywords.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omer.sahin\Desktop\repo\trendyolAutoBuy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omer.sahin\Desktop\Kişisel\repo\trendyolAutoBuy\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,30 +24,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Ayakkabı</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>Aranacak Kelime</t>
+  </si>
+  <si>
+    <t>Sleepy Bez 4 Numara</t>
+  </si>
+  <si>
+    <t>Sleepy Islak Mendil</t>
+  </si>
+  <si>
+    <t>Bebek Yürüteci</t>
+  </si>
+  <si>
+    <t>Kitap</t>
+  </si>
+  <si>
+    <t>Terlik</t>
+  </si>
+  <si>
+    <t>Bilgisayar</t>
+  </si>
+  <si>
+    <t>Laptop</t>
+  </si>
+  <si>
+    <t>Televizyon LCD</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy S10</t>
+  </si>
+  <si>
+    <t>iphone X</t>
+  </si>
+  <si>
+    <t>Bardak</t>
   </si>
   <si>
     <t>Kazak</t>
   </si>
   <si>
-    <t>Koltuk</t>
-  </si>
-  <si>
-    <t>Oyuncak Bebek</t>
-  </si>
-  <si>
-    <t>Kedi Maması</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ---------</t>
-  </si>
-  <si>
-    <t>Aranacak Kelime</t>
-  </si>
-  <si>
-    <t>Aselsan</t>
+    <t>Akülü Araba</t>
   </si>
 </sst>
 </file>
@@ -395,7 +413,7 @@
   <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,64 +423,73 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>5</v>
+      <c r="A8" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+      <c r="A13" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
+      <c r="A14" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>

</xml_diff>